<commit_message>
Versión Final de Documentos de SnoutPoint
</commit_message>
<xml_diff>
--- a/Proyecto/Quinto Incremento/Documentos/(SnoutPoint) - Asignación de Recursos y Tiempo.xlsx
+++ b/Proyecto/Quinto Incremento/Documentos/(SnoutPoint) - Asignación de Recursos y Tiempo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="20730" windowHeight="9555" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="20736" windowHeight="9552" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1° Inc - Recursos y Costos" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
     <author>tucompu</author>
   </authors>
   <commentList>
-    <comment ref="F11" authorId="0">
+    <comment ref="F12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="174">
   <si>
     <t>Id</t>
   </si>
@@ -674,9 +674,6 @@
     <t># de Hojas Recomendadas/ Número de funcionalidades</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Integrantes que Desarrollan la Tarea</t>
   </si>
   <si>
@@ -689,9 +686,6 @@
     <t>Enterprise Architech/Bizagi</t>
   </si>
   <si>
-    <t>Ruby On Rails/Sublime/Brackets/HTML 5 /MySQL</t>
-  </si>
-  <si>
     <t>EDCRC/Gerencia</t>
   </si>
   <si>
@@ -728,10 +722,22 @@
     <t>Generación de posibles requerimientos</t>
   </si>
   <si>
-    <t>Ruby On Rails/Sublime/Brackets/HTML 5 /SQLite</t>
-  </si>
-  <si>
     <t>Correcciones Basadas en la retroalimentacion</t>
+  </si>
+  <si>
+    <t>Publicidad y Mercadeo</t>
+  </si>
+  <si>
+    <t>Paint.net</t>
+  </si>
+  <si>
+    <t>Ruby On Rails/Cloud9/SQLite3/HTML 5</t>
+  </si>
+  <si>
+    <t>Costo del Cuarto Incremento</t>
+  </si>
+  <si>
+    <t>Costo del Quinto Incremento</t>
   </si>
 </sst>
 </file>
@@ -739,8 +745,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="166" formatCode="_-[$$-240A]\ * #,##0.00_ ;_-[$$-240A]\ * \-#,##0.00\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
@@ -1259,10 +1265,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1899,6 +1905,15 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1906,9 +1921,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2250,51 +2262,51 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K63" sqref="K63"/>
+      <selection pane="bottomRight" activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="1"/>
+    <col min="19" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="214" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="217" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="215"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
-      <c r="G1" s="215"/>
-      <c r="H1" s="215"/>
-      <c r="I1" s="215"/>
-      <c r="J1" s="215"/>
-      <c r="K1" s="215"/>
-      <c r="L1" s="216"/>
-    </row>
-    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="218"/>
+      <c r="L1" s="219"/>
+    </row>
+    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="83" t="s">
         <v>0</v>
       </c>
@@ -2389,7 +2401,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="189">
         <v>2</v>
       </c>
@@ -2434,7 +2446,7 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32">
         <v>3</v>
       </c>
@@ -2479,7 +2491,7 @@
       <c r="Q5" s="10"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32">
         <v>4</v>
       </c>
@@ -2524,7 +2536,7 @@
       <c r="Q6" s="11"/>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32">
         <v>5</v>
       </c>
@@ -2563,7 +2575,7 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32">
         <v>6</v>
       </c>
@@ -2601,7 +2613,7 @@
       </c>
       <c r="M8" s="44"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32">
         <v>7</v>
       </c>
@@ -2638,7 +2650,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32">
         <v>8</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32">
         <v>9</v>
       </c>
@@ -2712,7 +2724,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
         <v>10</v>
       </c>
@@ -2749,7 +2761,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32">
         <v>11</v>
       </c>
@@ -2786,7 +2798,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32">
         <v>12</v>
       </c>
@@ -2823,7 +2835,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
         <v>13</v>
       </c>
@@ -2860,7 +2872,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32">
         <v>14</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -3176,7 +3188,7 @@
         <v>1764.3229166666667</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -3212,7 +3224,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <v>24</v>
       </c>
@@ -3302,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>27</v>
       </c>
@@ -3342,7 +3354,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>28</v>
       </c>
@@ -3378,7 +3390,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>29</v>
       </c>
@@ -3412,7 +3424,7 @@
         <v>28229.166666666668</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -3446,7 +3458,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -3486,7 +3498,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -3510,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>33</v>
       </c>
@@ -3542,7 +3554,7 @@
         <v>232890.625</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="22">
         <v>34</v>
       </c>
@@ -3582,7 +3594,7 @@
         <v>105859.375</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22">
         <v>35</v>
       </c>
@@ -3622,7 +3634,7 @@
         <v>127031.25</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>36</v>
       </c>
@@ -3660,7 +3672,7 @@
         <v>10585.9375</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22">
         <v>37</v>
       </c>
@@ -3693,16 +3705,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O39" s="217" t="s">
+      <c r="O39" s="216" t="s">
         <v>115</v>
       </c>
-      <c r="P39" s="217"/>
-      <c r="Q39" s="217" t="s">
+      <c r="P39" s="216"/>
+      <c r="Q39" s="216" t="s">
         <v>116</v>
       </c>
-      <c r="R39" s="217"/>
-    </row>
-    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R39" s="216"/>
+    </row>
+    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>38</v>
       </c>
@@ -3741,12 +3753,12 @@
       <c r="P40" s="46">
         <v>42042</v>
       </c>
-      <c r="Q40" s="217">
+      <c r="Q40" s="216">
         <v>1</v>
       </c>
-      <c r="R40" s="217"/>
-    </row>
-    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R40" s="216"/>
+    </row>
+    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
         <v>39</v>
       </c>
@@ -3785,12 +3797,12 @@
       <c r="P41" s="46">
         <v>42049</v>
       </c>
-      <c r="Q41" s="217">
+      <c r="Q41" s="216">
         <v>2</v>
       </c>
-      <c r="R41" s="217"/>
-    </row>
-    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R41" s="216"/>
+    </row>
+    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>40</v>
       </c>
@@ -3833,12 +3845,12 @@
       <c r="P42" s="46">
         <v>42056</v>
       </c>
-      <c r="Q42" s="217">
+      <c r="Q42" s="216">
         <v>3</v>
       </c>
-      <c r="R42" s="217"/>
-    </row>
-    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R42" s="216"/>
+    </row>
+    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>41</v>
       </c>
@@ -3871,12 +3883,12 @@
       <c r="P43" s="46">
         <v>42063</v>
       </c>
-      <c r="Q43" s="217">
+      <c r="Q43" s="216">
         <v>4</v>
       </c>
-      <c r="R43" s="217"/>
-    </row>
-    <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R43" s="216"/>
+    </row>
+    <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>42</v>
       </c>
@@ -3921,12 +3933,12 @@
       <c r="P44" s="46">
         <v>42070</v>
       </c>
-      <c r="Q44" s="217">
+      <c r="Q44" s="216">
         <v>5</v>
       </c>
-      <c r="R44" s="217"/>
-    </row>
-    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R44" s="216"/>
+    </row>
+    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="22">
         <v>43</v>
       </c>
@@ -3971,12 +3983,12 @@
       <c r="P45" s="46">
         <v>42077</v>
       </c>
-      <c r="Q45" s="217">
+      <c r="Q45" s="216">
         <v>6</v>
       </c>
-      <c r="R45" s="217"/>
-    </row>
-    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R45" s="216"/>
+    </row>
+    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -4005,12 +4017,12 @@
       <c r="P46" s="46">
         <v>42084</v>
       </c>
-      <c r="Q46" s="217">
+      <c r="Q46" s="216">
         <v>7</v>
       </c>
-      <c r="R46" s="217"/>
-    </row>
-    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R46" s="216"/>
+    </row>
+    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>45</v>
       </c>
@@ -4055,12 +4067,12 @@
       <c r="P47" s="46">
         <v>42091</v>
       </c>
-      <c r="Q47" s="217">
+      <c r="Q47" s="216">
         <v>8</v>
       </c>
-      <c r="R47" s="217"/>
-    </row>
-    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R47" s="216"/>
+    </row>
+    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>46</v>
       </c>
@@ -4095,12 +4107,12 @@
       <c r="P48" s="46">
         <v>42098</v>
       </c>
-      <c r="Q48" s="217">
+      <c r="Q48" s="216">
         <v>9</v>
       </c>
-      <c r="R48" s="217"/>
-    </row>
-    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R48" s="216"/>
+    </row>
+    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22">
         <v>47</v>
       </c>
@@ -4145,12 +4157,12 @@
       <c r="P49" s="46">
         <v>42105</v>
       </c>
-      <c r="Q49" s="217">
+      <c r="Q49" s="216">
         <v>10</v>
       </c>
-      <c r="R49" s="217"/>
-    </row>
-    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R49" s="216"/>
+    </row>
+    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
         <v>48</v>
       </c>
@@ -4195,12 +4207,12 @@
       <c r="P50" s="46">
         <v>42112</v>
       </c>
-      <c r="Q50" s="217">
+      <c r="Q50" s="216">
         <v>11</v>
       </c>
-      <c r="R50" s="217"/>
-    </row>
-    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R50" s="216"/>
+    </row>
+    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>49</v>
       </c>
@@ -4231,12 +4243,12 @@
       <c r="P51" s="46">
         <v>42119</v>
       </c>
-      <c r="Q51" s="217">
+      <c r="Q51" s="216">
         <v>12</v>
       </c>
-      <c r="R51" s="217"/>
-    </row>
-    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R51" s="216"/>
+    </row>
+    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22">
         <v>50</v>
       </c>
@@ -4281,12 +4293,12 @@
       <c r="P52" s="46">
         <v>42126</v>
       </c>
-      <c r="Q52" s="217">
+      <c r="Q52" s="216">
         <v>13</v>
       </c>
-      <c r="R52" s="217"/>
-    </row>
-    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R52" s="216"/>
+    </row>
+    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="22">
         <v>51</v>
       </c>
@@ -4331,12 +4343,12 @@
       <c r="P53" s="46">
         <v>42133</v>
       </c>
-      <c r="Q53" s="217">
+      <c r="Q53" s="216">
         <v>14</v>
       </c>
-      <c r="R53" s="217"/>
-    </row>
-    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R53" s="216"/>
+    </row>
+    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22">
         <v>52</v>
       </c>
@@ -4381,12 +4393,12 @@
       <c r="P54" s="46">
         <v>42140</v>
       </c>
-      <c r="Q54" s="217">
+      <c r="Q54" s="216">
         <v>15</v>
       </c>
-      <c r="R54" s="217"/>
-    </row>
-    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R54" s="216"/>
+    </row>
+    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="22">
         <v>53</v>
       </c>
@@ -4431,12 +4443,12 @@
       <c r="P55" s="46">
         <v>42147</v>
       </c>
-      <c r="Q55" s="217">
+      <c r="Q55" s="216">
         <v>16</v>
       </c>
-      <c r="R55" s="217"/>
-    </row>
-    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R55" s="216"/>
+    </row>
+    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>54</v>
       </c>
@@ -4465,12 +4477,12 @@
       <c r="P56" s="46">
         <v>42154</v>
       </c>
-      <c r="Q56" s="217">
+      <c r="Q56" s="216">
         <v>17</v>
       </c>
-      <c r="R56" s="217"/>
-    </row>
-    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R56" s="216"/>
+    </row>
+    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -4510,7 +4522,7 @@
         <v>49401.041666666672</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>56</v>
       </c>
@@ -4556,7 +4568,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>57</v>
       </c>
@@ -4602,7 +4614,7 @@
         <v>1693750</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>58</v>
       </c>
@@ -4633,7 +4645,7 @@
         <v>56458.333333333336</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -4680,7 +4692,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>60</v>
       </c>
@@ -4720,7 +4732,7 @@
         <v>42343.75</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>61</v>
       </c>
@@ -4760,7 +4772,7 @@
         <v>70572.916666666672</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -4929,26 +4941,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="Q51:R51"/>
     <mergeCell ref="Q52:R52"/>
     <mergeCell ref="Q53:R53"/>
     <mergeCell ref="Q54:R54"/>
     <mergeCell ref="Q55:R55"/>
     <mergeCell ref="Q56:R56"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="Q51:R51"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="Q41:R41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4960,49 +4972,49 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="50" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="50" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="50" customWidth="1"/>
     <col min="7" max="7" width="16" style="50" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="50" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="50" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="50" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="50" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="50"/>
+    <col min="19" max="16384" width="11.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="218" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="220" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
-      <c r="H1" s="219"/>
-      <c r="I1" s="219"/>
-      <c r="J1" s="219"/>
-      <c r="K1" s="219"/>
-      <c r="L1" s="220"/>
-    </row>
-    <row r="2" spans="1:18" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="222"/>
+    </row>
+    <row r="2" spans="1:18" ht="77.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="79" t="s">
         <v>0</v>
       </c>
@@ -5031,7 +5043,7 @@
         <v>2</v>
       </c>
       <c r="J2" s="79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K2" s="80" t="s">
         <v>91</v>
@@ -5046,7 +5058,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -5094,7 +5106,7 @@
       <c r="Q3" s="54"/>
       <c r="R3" s="55"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61">
         <v>2</v>
       </c>
@@ -5142,7 +5154,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
         <v>3</v>
       </c>
@@ -5223,7 +5235,7 @@
       <c r="Q6" s="64"/>
       <c r="R6" s="65"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="87">
         <v>5</v>
       </c>
@@ -5253,10 +5265,10 @@
         <v>42114</v>
       </c>
       <c r="J7" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K7" s="61" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="L7" s="62">
         <f t="shared" si="0"/>
@@ -5265,12 +5277,12 @@
       <c r="Q7" s="66"/>
       <c r="R7" s="67"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="87">
         <v>6</v>
       </c>
       <c r="B8" s="76" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C8" s="61">
         <v>10</v>
@@ -5312,12 +5324,12 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87">
         <v>7</v>
       </c>
       <c r="B9" s="76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C9" s="61">
         <v>15</v>
@@ -5342,7 +5354,7 @@
         <v>42098</v>
       </c>
       <c r="J9" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K9" s="61" t="s">
         <v>10</v>
@@ -5358,7 +5370,7 @@
         <v>42091</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="117">
         <v>8</v>
       </c>
@@ -5389,7 +5401,7 @@
         <v>42098</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>9</v>
       </c>
@@ -5412,7 +5424,7 @@
         <v>42091</v>
       </c>
       <c r="J11" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K11" s="61"/>
       <c r="L11" s="53">
@@ -5449,10 +5461,10 @@
         <v>42111</v>
       </c>
       <c r="J12" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12" s="61" t="s">
         <v>155</v>
-      </c>
-      <c r="K12" s="61" t="s">
-        <v>156</v>
       </c>
       <c r="L12" s="53">
         <f t="shared" si="0"/>
@@ -5465,7 +5477,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="38.450000000000003" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="87">
         <v>11</v>
       </c>
@@ -5498,7 +5510,7 @@
         <v>70</v>
       </c>
       <c r="K13" s="61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L13" s="53">
         <f>$O$6*F13</f>
@@ -5511,7 +5523,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="87">
         <v>12</v>
       </c>
@@ -5537,7 +5549,7 @@
         <v>70</v>
       </c>
       <c r="K14" s="61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L14" s="53">
         <f t="shared" si="0"/>
@@ -5550,7 +5562,7 @@
         <v>42126</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117">
         <v>13</v>
       </c>
@@ -5589,7 +5601,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="117">
         <v>14</v>
       </c>
@@ -5612,10 +5624,10 @@
         <v>42111</v>
       </c>
       <c r="J16" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="117" t="s">
         <v>158</v>
-      </c>
-      <c r="K16" s="117" t="s">
-        <v>160</v>
       </c>
       <c r="L16" s="121">
         <f t="shared" si="0"/>
@@ -5628,7 +5640,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="97"/>
       <c r="B17" s="91"/>
       <c r="C17" s="91"/>
@@ -5646,7 +5658,7 @@
       <c r="I17" s="93"/>
       <c r="J17" s="92"/>
       <c r="K17" s="89" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L17" s="90">
         <f>SUM(L61:L67)+L59+L58+L57+L55+L54+L53+L52+L50+L49+L48+L47+L45+L44+L43+L42+L38+L37+L36+L33+L32+L31+L30+L29+L25+L24+L22+L21+L20+L19+L18+SUM(L3:L14)</f>
@@ -5659,7 +5671,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="97"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
@@ -5679,7 +5691,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="97"/>
       <c r="B19" s="91"/>
       <c r="C19" s="92"/>
@@ -5693,7 +5705,7 @@
       <c r="K19" s="92"/>
       <c r="L19" s="94"/>
     </row>
-    <row r="20" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="97"/>
       <c r="B20" s="95"/>
       <c r="C20" s="92"/>
@@ -5707,7 +5719,7 @@
       <c r="K20" s="92"/>
       <c r="L20" s="94"/>
     </row>
-    <row r="21" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="97"/>
       <c r="B21" s="96"/>
       <c r="C21" s="92"/>
@@ -5727,7 +5739,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="97"/>
       <c r="B22" s="209"/>
       <c r="C22" s="92"/>
@@ -5748,7 +5760,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A23" s="92"/>
       <c r="B23" s="96"/>
       <c r="C23" s="92"/>
@@ -5769,7 +5781,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="92"/>
       <c r="B24" s="96"/>
       <c r="C24" s="92"/>
@@ -5790,7 +5802,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="97"/>
       <c r="B25" s="211"/>
       <c r="C25" s="91"/>
@@ -5811,7 +5823,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="97"/>
       <c r="B26" s="213"/>
       <c r="C26" s="92"/>
@@ -5826,7 +5838,7 @@
       <c r="L26" s="212"/>
       <c r="M26" s="91"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="97"/>
       <c r="B27" s="213"/>
       <c r="C27" s="92"/>
@@ -5841,7 +5853,7 @@
       <c r="L27" s="212"/>
       <c r="M27" s="91"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="92"/>
       <c r="B28" s="96"/>
       <c r="C28" s="92"/>
@@ -5856,7 +5868,7 @@
       <c r="L28" s="94"/>
       <c r="M28" s="91"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="92"/>
       <c r="B29" s="96"/>
       <c r="C29" s="92"/>
@@ -5871,7 +5883,7 @@
       <c r="L29" s="94"/>
       <c r="M29" s="91"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="92"/>
       <c r="B30" s="96"/>
       <c r="C30" s="92"/>
@@ -5886,7 +5898,7 @@
       <c r="L30" s="94"/>
       <c r="M30" s="91"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="92"/>
       <c r="B31" s="96"/>
       <c r="C31" s="92"/>
@@ -5900,7 +5912,7 @@
       <c r="K31" s="92"/>
       <c r="L31" s="94"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="92"/>
       <c r="B32" s="96"/>
       <c r="C32" s="92"/>
@@ -5914,7 +5926,7 @@
       <c r="K32" s="92"/>
       <c r="L32" s="94"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="92"/>
       <c r="B33" s="96"/>
       <c r="C33" s="92"/>
@@ -5928,7 +5940,7 @@
       <c r="K33" s="92"/>
       <c r="L33" s="94"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="92"/>
       <c r="B34" s="96"/>
       <c r="C34" s="92"/>
@@ -5942,7 +5954,7 @@
       <c r="K34" s="92"/>
       <c r="L34" s="94"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="92"/>
       <c r="B35" s="95"/>
       <c r="C35" s="92"/>
@@ -5956,7 +5968,7 @@
       <c r="K35" s="92"/>
       <c r="L35" s="94"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="92"/>
       <c r="B36" s="96"/>
       <c r="C36" s="92"/>
@@ -5970,7 +5982,7 @@
       <c r="K36" s="92"/>
       <c r="L36" s="94"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="92"/>
       <c r="B37" s="96"/>
       <c r="C37" s="92"/>
@@ -5984,7 +5996,7 @@
       <c r="K37" s="92"/>
       <c r="L37" s="94"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="92"/>
       <c r="B38" s="96"/>
       <c r="C38" s="92"/>
@@ -5998,7 +6010,7 @@
       <c r="K38" s="92"/>
       <c r="L38" s="94"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="92"/>
       <c r="B39" s="96"/>
       <c r="C39" s="92"/>
@@ -6012,7 +6024,7 @@
       <c r="K39" s="92"/>
       <c r="L39" s="94"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="92"/>
       <c r="B40" s="96"/>
       <c r="C40" s="92"/>
@@ -6026,7 +6038,7 @@
       <c r="K40" s="92"/>
       <c r="L40" s="94"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="92"/>
       <c r="B41" s="96"/>
       <c r="C41" s="92"/>
@@ -6040,7 +6052,7 @@
       <c r="K41" s="92"/>
       <c r="L41" s="94"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="92"/>
       <c r="B42" s="96"/>
       <c r="C42" s="92"/>
@@ -6054,7 +6066,7 @@
       <c r="K42" s="92"/>
       <c r="L42" s="94"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="92"/>
       <c r="B43" s="96"/>
       <c r="C43" s="92"/>
@@ -6068,7 +6080,7 @@
       <c r="K43" s="92"/>
       <c r="L43" s="94"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="92"/>
       <c r="B44" s="96"/>
       <c r="C44" s="92"/>
@@ -6082,7 +6094,7 @@
       <c r="K44" s="92"/>
       <c r="L44" s="94"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="92"/>
       <c r="B45" s="96"/>
       <c r="C45" s="92"/>
@@ -6096,7 +6108,7 @@
       <c r="K45" s="92"/>
       <c r="L45" s="94"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="92"/>
       <c r="B46" s="96"/>
       <c r="C46" s="92"/>
@@ -6110,7 +6122,7 @@
       <c r="K46" s="92"/>
       <c r="L46" s="94"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="92"/>
       <c r="B47" s="96"/>
       <c r="C47" s="92"/>
@@ -6124,7 +6136,7 @@
       <c r="K47" s="92"/>
       <c r="L47" s="94"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="92"/>
       <c r="B48" s="95"/>
       <c r="C48" s="92"/>
@@ -6138,7 +6150,7 @@
       <c r="K48" s="92"/>
       <c r="L48" s="94"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="92"/>
       <c r="B49" s="96"/>
       <c r="C49" s="92"/>
@@ -6152,7 +6164,7 @@
       <c r="K49" s="92"/>
       <c r="L49" s="94"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="92"/>
       <c r="B50" s="96"/>
       <c r="C50" s="92"/>
@@ -6166,7 +6178,7 @@
       <c r="K50" s="92"/>
       <c r="L50" s="94"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="92"/>
       <c r="B51" s="96"/>
       <c r="C51" s="92"/>
@@ -6180,7 +6192,7 @@
       <c r="K51" s="92"/>
       <c r="L51" s="94"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="92"/>
       <c r="B52" s="96"/>
       <c r="C52" s="92"/>
@@ -6194,7 +6206,7 @@
       <c r="K52" s="92"/>
       <c r="L52" s="94"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="92"/>
       <c r="B53" s="96"/>
       <c r="C53" s="92"/>
@@ -6208,7 +6220,7 @@
       <c r="K53" s="92"/>
       <c r="L53" s="94"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="92"/>
       <c r="B54" s="96"/>
       <c r="C54" s="92"/>
@@ -6222,7 +6234,7 @@
       <c r="K54" s="92"/>
       <c r="L54" s="94"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="92"/>
       <c r="B55" s="96"/>
       <c r="C55" s="92"/>
@@ -6236,7 +6248,7 @@
       <c r="K55" s="92"/>
       <c r="L55" s="94"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="92"/>
       <c r="B56" s="96"/>
       <c r="C56" s="92"/>
@@ -6250,7 +6262,7 @@
       <c r="K56" s="92"/>
       <c r="L56" s="94"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="92"/>
       <c r="B57" s="96"/>
       <c r="C57" s="92"/>
@@ -6264,7 +6276,7 @@
       <c r="K57" s="92"/>
       <c r="L57" s="94"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="92"/>
       <c r="B58" s="96"/>
       <c r="C58" s="92"/>
@@ -6278,7 +6290,7 @@
       <c r="K58" s="92"/>
       <c r="L58" s="94"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="92"/>
       <c r="B59" s="96"/>
       <c r="C59" s="92"/>
@@ -6292,7 +6304,7 @@
       <c r="K59" s="92"/>
       <c r="L59" s="94"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="92"/>
       <c r="B60" s="96"/>
       <c r="C60" s="92"/>
@@ -6306,7 +6318,7 @@
       <c r="K60" s="92"/>
       <c r="L60" s="94"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="92"/>
       <c r="B61" s="92"/>
       <c r="C61" s="92"/>
@@ -6320,7 +6332,7 @@
       <c r="K61" s="92"/>
       <c r="L61" s="94"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="92"/>
       <c r="B62" s="92"/>
       <c r="C62" s="92"/>
@@ -6334,7 +6346,7 @@
       <c r="K62" s="92"/>
       <c r="L62" s="94"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="92"/>
       <c r="B63" s="92"/>
       <c r="C63" s="92"/>
@@ -6348,7 +6360,7 @@
       <c r="K63" s="92"/>
       <c r="L63" s="94"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="92"/>
       <c r="B64" s="92"/>
       <c r="C64" s="92"/>
@@ -6362,7 +6374,7 @@
       <c r="K64" s="92"/>
       <c r="L64" s="94"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="92"/>
       <c r="B65" s="92"/>
       <c r="C65" s="92"/>
@@ -6376,7 +6388,7 @@
       <c r="K65" s="92"/>
       <c r="L65" s="94"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="92"/>
       <c r="B66" s="92"/>
       <c r="C66" s="92"/>
@@ -6390,7 +6402,7 @@
       <c r="K66" s="92"/>
       <c r="L66" s="94"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="92"/>
       <c r="B67" s="92"/>
       <c r="C67" s="92"/>
@@ -6404,19 +6416,19 @@
       <c r="K67" s="92"/>
       <c r="L67" s="94"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="92"/>
       <c r="B68" s="91"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="91"/>
       <c r="B69" s="91"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="91"/>
       <c r="B70" s="91"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="91"/>
       <c r="B71" s="91"/>
     </row>
@@ -6433,48 +6445,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" style="50" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="50" customWidth="1"/>
-    <col min="5" max="6" width="16.5703125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" style="50" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="50" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="50" customWidth="1"/>
+    <col min="5" max="6" width="16.5546875" style="50" customWidth="1"/>
     <col min="7" max="7" width="16" style="50" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" style="50" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="50"/>
+    <col min="19" max="16384" width="11.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="221" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="223" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221"/>
-      <c r="J1" s="221"/>
-      <c r="K1" s="221"/>
-      <c r="L1" s="221"/>
-    </row>
-    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="223"/>
+      <c r="K1" s="223"/>
+      <c r="L1" s="223"/>
+    </row>
+    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="116" t="s">
         <v>0</v>
       </c>
@@ -6518,12 +6530,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>1</v>
       </c>
       <c r="B3" s="122" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -6583,12 +6595,12 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
         <v>3</v>
       </c>
       <c r="B5" s="203" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="61">
         <v>5</v>
@@ -6613,10 +6625,10 @@
         <v>42112</v>
       </c>
       <c r="J5" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K5" s="61" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L5" s="62">
         <f t="shared" si="0"/>
@@ -6632,7 +6644,7 @@
       <c r="Q5" s="63"/>
       <c r="R5" s="60"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -6662,10 +6674,10 @@
         <v>42114</v>
       </c>
       <c r="J6" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K6" s="61" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L6" s="62">
         <f t="shared" si="0"/>
@@ -6725,7 +6737,7 @@
       <c r="Q7" s="201"/>
       <c r="R7" s="202"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="61">
         <v>6</v>
       </c>
@@ -6769,7 +6781,7 @@
       <c r="Q8" s="201"/>
       <c r="R8" s="202"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87">
         <v>7</v>
       </c>
@@ -6799,7 +6811,7 @@
         <v>42098</v>
       </c>
       <c r="J9" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K9" s="61" t="s">
         <v>10</v>
@@ -6861,7 +6873,7 @@
         <v>42107</v>
       </c>
       <c r="J11" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K11" s="61"/>
       <c r="L11" s="62">
@@ -6898,10 +6910,10 @@
         <v>42107</v>
       </c>
       <c r="J12" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K12" s="61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L12" s="62">
         <f t="shared" si="2"/>
@@ -6937,10 +6949,10 @@
         <v>42112</v>
       </c>
       <c r="J13" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="K13" s="61" t="s">
         <v>155</v>
-      </c>
-      <c r="K13" s="61" t="s">
-        <v>156</v>
       </c>
       <c r="L13" s="62">
         <f t="shared" si="2"/>
@@ -6986,7 +6998,7 @@
         <v>70</v>
       </c>
       <c r="K14" s="61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L14" s="62">
         <f t="shared" si="2"/>
@@ -6999,7 +7011,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="51">
         <v>13</v>
       </c>
@@ -7022,10 +7034,10 @@
         <v>42115</v>
       </c>
       <c r="J15" s="61" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K15" s="61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L15" s="62">
         <f t="shared" si="2"/>
@@ -7038,7 +7050,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="61">
         <v>14</v>
       </c>
@@ -7122,7 +7134,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="117">
         <v>16</v>
       </c>
@@ -7148,7 +7160,7 @@
         <v>84</v>
       </c>
       <c r="K18" s="117" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L18" s="121">
         <f t="shared" si="2"/>
@@ -7161,7 +7173,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="97"/>
       <c r="F19" s="50">
         <f>SUM(F3:F18)</f>
@@ -7172,7 +7184,7 @@
         <v>203</v>
       </c>
       <c r="K19" s="129" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L19" s="75">
         <f>SUM(L3:L18)</f>
@@ -7186,7 +7198,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="97"/>
       <c r="B20" s="125"/>
       <c r="C20" s="97"/>
@@ -7207,7 +7219,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="97"/>
       <c r="B21" s="125"/>
       <c r="C21" s="97"/>
@@ -7224,7 +7236,7 @@
       <c r="N21" s="101"/>
       <c r="O21" s="101"/>
     </row>
-    <row r="22" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="97"/>
       <c r="B22" s="125"/>
       <c r="C22" s="97"/>
@@ -7241,7 +7253,7 @@
       <c r="N22" s="101"/>
       <c r="O22" s="101"/>
     </row>
-    <row r="23" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="97"/>
       <c r="B23" s="125"/>
       <c r="C23" s="97"/>
@@ -7262,7 +7274,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="97"/>
       <c r="B24" s="125"/>
       <c r="C24" s="97"/>
@@ -7283,7 +7295,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A25" s="97"/>
       <c r="B25" s="125"/>
       <c r="C25" s="97"/>
@@ -7304,7 +7316,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="97"/>
       <c r="B26" s="125"/>
       <c r="C26" s="97"/>
@@ -7325,7 +7337,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="97"/>
       <c r="B27" s="125"/>
       <c r="C27" s="97"/>
@@ -7346,7 +7358,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="97"/>
       <c r="B28" s="125"/>
       <c r="C28" s="97"/>
@@ -7363,7 +7375,7 @@
       <c r="N28" s="101"/>
       <c r="O28" s="101"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="97"/>
       <c r="B29" s="125"/>
       <c r="C29" s="97"/>
@@ -7380,7 +7392,7 @@
       <c r="N29" s="101"/>
       <c r="O29" s="101"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="97"/>
       <c r="B30" s="125"/>
       <c r="C30" s="97"/>
@@ -7397,7 +7409,7 @@
       <c r="N30" s="101"/>
       <c r="O30" s="101"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="97"/>
       <c r="B31" s="125"/>
       <c r="C31" s="97"/>
@@ -7414,7 +7426,7 @@
       <c r="N31" s="101"/>
       <c r="O31" s="101"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="97"/>
       <c r="B32" s="125"/>
       <c r="C32" s="97"/>
@@ -7431,7 +7443,7 @@
       <c r="N32" s="101"/>
       <c r="O32" s="101"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="97"/>
       <c r="B33" s="125"/>
       <c r="C33" s="97"/>
@@ -7448,7 +7460,7 @@
       <c r="N33" s="101"/>
       <c r="O33" s="101"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="97"/>
       <c r="B34" s="125"/>
       <c r="C34" s="97"/>
@@ -7465,7 +7477,7 @@
       <c r="N34" s="101"/>
       <c r="O34" s="101"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="97"/>
       <c r="B35" s="125"/>
       <c r="C35" s="97"/>
@@ -7482,7 +7494,7 @@
       <c r="N35" s="101"/>
       <c r="O35" s="101"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="97"/>
       <c r="B36" s="125"/>
       <c r="C36" s="97"/>
@@ -7499,7 +7511,7 @@
       <c r="N36" s="101"/>
       <c r="O36" s="101"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="97"/>
       <c r="B37" s="125"/>
       <c r="C37" s="97"/>
@@ -7516,7 +7528,7 @@
       <c r="N37" s="101"/>
       <c r="O37" s="101"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="97"/>
       <c r="B38" s="125"/>
       <c r="C38" s="97"/>
@@ -7533,7 +7545,7 @@
       <c r="N38" s="101"/>
       <c r="O38" s="101"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="97"/>
       <c r="B39" s="125"/>
       <c r="C39" s="97"/>
@@ -7550,7 +7562,7 @@
       <c r="N39" s="101"/>
       <c r="O39" s="101"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="97"/>
       <c r="B40" s="125"/>
       <c r="C40" s="97"/>
@@ -7567,7 +7579,7 @@
       <c r="N40" s="101"/>
       <c r="O40" s="101"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="97"/>
       <c r="B41" s="125"/>
       <c r="C41" s="97"/>
@@ -7584,7 +7596,7 @@
       <c r="N41" s="101"/>
       <c r="O41" s="101"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="97"/>
       <c r="B42" s="125"/>
       <c r="C42" s="97"/>
@@ -7601,7 +7613,7 @@
       <c r="N42" s="101"/>
       <c r="O42" s="101"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="97"/>
       <c r="B43" s="125"/>
       <c r="C43" s="97"/>
@@ -7618,7 +7630,7 @@
       <c r="N43" s="101"/>
       <c r="O43" s="101"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="97"/>
       <c r="B44" s="125"/>
       <c r="C44" s="97"/>
@@ -7635,7 +7647,7 @@
       <c r="N44" s="101"/>
       <c r="O44" s="101"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="97"/>
       <c r="B45" s="125"/>
       <c r="C45" s="97"/>
@@ -7652,7 +7664,7 @@
       <c r="N45" s="101"/>
       <c r="O45" s="101"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="97"/>
       <c r="B46" s="125"/>
       <c r="C46" s="97"/>
@@ -7669,7 +7681,7 @@
       <c r="N46" s="101"/>
       <c r="O46" s="101"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="97"/>
       <c r="B47" s="125"/>
       <c r="C47" s="97"/>
@@ -7686,7 +7698,7 @@
       <c r="N47" s="101"/>
       <c r="O47" s="101"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="97"/>
       <c r="B48" s="125"/>
       <c r="C48" s="97"/>
@@ -7703,7 +7715,7 @@
       <c r="N48" s="101"/>
       <c r="O48" s="101"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="97"/>
       <c r="B49" s="125"/>
       <c r="C49" s="97"/>
@@ -7720,7 +7732,7 @@
       <c r="N49" s="101"/>
       <c r="O49" s="101"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="97"/>
       <c r="B50" s="125"/>
       <c r="C50" s="97"/>
@@ -7737,7 +7749,7 @@
       <c r="N50" s="101"/>
       <c r="O50" s="101"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="97"/>
       <c r="B51" s="125"/>
       <c r="C51" s="97"/>
@@ -7754,7 +7766,7 @@
       <c r="N51" s="101"/>
       <c r="O51" s="101"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="97"/>
       <c r="B52" s="125"/>
       <c r="C52" s="97"/>
@@ -7771,7 +7783,7 @@
       <c r="N52" s="101"/>
       <c r="O52" s="101"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="97"/>
       <c r="B53" s="125"/>
       <c r="C53" s="97"/>
@@ -7788,7 +7800,7 @@
       <c r="N53" s="101"/>
       <c r="O53" s="101"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="97"/>
       <c r="B54" s="125"/>
       <c r="C54" s="97"/>
@@ -7805,7 +7817,7 @@
       <c r="N54" s="101"/>
       <c r="O54" s="101"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="97"/>
       <c r="B55" s="125"/>
       <c r="C55" s="97"/>
@@ -7822,7 +7834,7 @@
       <c r="N55" s="101"/>
       <c r="O55" s="101"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="97"/>
       <c r="B56" s="125"/>
       <c r="C56" s="97"/>
@@ -7839,7 +7851,7 @@
       <c r="N56" s="101"/>
       <c r="O56" s="101"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="97"/>
       <c r="B57" s="125"/>
       <c r="C57" s="97"/>
@@ -7856,7 +7868,7 @@
       <c r="N57" s="101"/>
       <c r="O57" s="101"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="97"/>
       <c r="B58" s="125"/>
       <c r="C58" s="97"/>
@@ -7873,7 +7885,7 @@
       <c r="N58" s="101"/>
       <c r="O58" s="101"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="97"/>
       <c r="B59" s="125"/>
       <c r="C59" s="97"/>
@@ -7890,7 +7902,7 @@
       <c r="N59" s="101"/>
       <c r="O59" s="101"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="97"/>
       <c r="B60" s="125"/>
       <c r="C60" s="97"/>
@@ -7907,7 +7919,7 @@
       <c r="N60" s="101"/>
       <c r="O60" s="101"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="97"/>
       <c r="B61" s="125"/>
       <c r="C61" s="97"/>
@@ -7924,7 +7936,7 @@
       <c r="N61" s="101"/>
       <c r="O61" s="101"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="97"/>
       <c r="B62" s="125"/>
       <c r="C62" s="97"/>
@@ -7941,7 +7953,7 @@
       <c r="N62" s="101"/>
       <c r="O62" s="101"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="97"/>
       <c r="B63" s="97"/>
       <c r="C63" s="97"/>
@@ -7958,7 +7970,7 @@
       <c r="N63" s="101"/>
       <c r="O63" s="101"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="97"/>
       <c r="B64" s="97"/>
       <c r="C64" s="97"/>
@@ -7975,7 +7987,7 @@
       <c r="N64" s="101"/>
       <c r="O64" s="101"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="97"/>
       <c r="B65" s="97"/>
       <c r="C65" s="97"/>
@@ -7992,7 +8004,7 @@
       <c r="N65" s="101"/>
       <c r="O65" s="101"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="97"/>
       <c r="B66" s="97"/>
       <c r="C66" s="97"/>
@@ -8009,7 +8021,7 @@
       <c r="N66" s="101"/>
       <c r="O66" s="101"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="97"/>
       <c r="B67" s="97"/>
       <c r="C67" s="97"/>
@@ -8026,7 +8038,7 @@
       <c r="N67" s="101"/>
       <c r="O67" s="101"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="97"/>
       <c r="B68" s="97"/>
       <c r="C68" s="97"/>
@@ -8043,7 +8055,7 @@
       <c r="N68" s="101"/>
       <c r="O68" s="101"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="97"/>
       <c r="B69" s="97"/>
       <c r="C69" s="97"/>
@@ -8060,7 +8072,7 @@
       <c r="N69" s="101"/>
       <c r="O69" s="101"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="97"/>
       <c r="B70" s="97"/>
       <c r="C70" s="97"/>
@@ -8077,7 +8089,7 @@
       <c r="N70" s="101"/>
       <c r="O70" s="101"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="97"/>
       <c r="B71" s="97"/>
       <c r="C71" s="97"/>
@@ -8094,7 +8106,7 @@
       <c r="N71" s="101"/>
       <c r="O71" s="101"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="97"/>
       <c r="B72" s="97"/>
       <c r="C72" s="97"/>
@@ -8111,7 +8123,7 @@
       <c r="N72" s="101"/>
       <c r="O72" s="101"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="97"/>
       <c r="B73" s="97"/>
       <c r="C73" s="97"/>
@@ -8128,7 +8140,7 @@
       <c r="N73" s="101"/>
       <c r="O73" s="101"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="97"/>
       <c r="B74" s="97"/>
       <c r="C74" s="101"/>
@@ -8159,49 +8171,49 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="K16" sqref="K16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="50" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="50" customWidth="1"/>
     <col min="4" max="4" width="19" style="50" customWidth="1"/>
     <col min="5" max="5" width="16" style="50" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="50" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="50" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="50" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="50" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="50" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="50" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="50" customWidth="1"/>
     <col min="10" max="10" width="29" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="50"/>
+    <col min="19" max="16384" width="11.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="218" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="220" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
-      <c r="H1" s="219"/>
-      <c r="I1" s="219"/>
-      <c r="J1" s="219"/>
-      <c r="K1" s="219"/>
-      <c r="L1" s="220"/>
-    </row>
-    <row r="2" spans="1:18" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="222"/>
+    </row>
+    <row r="2" spans="1:18" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="79" t="s">
         <v>0</v>
       </c>
@@ -8209,7 +8221,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D2" s="81" t="s">
         <v>102</v>
@@ -8245,7 +8257,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -8258,8 +8270,8 @@
       <c r="F3" s="61">
         <v>2</v>
       </c>
-      <c r="G3" s="61" t="s">
-        <v>152</v>
+      <c r="G3" s="61">
+        <v>2</v>
       </c>
       <c r="H3" s="69">
         <v>42118</v>
@@ -8286,7 +8298,7 @@
       <c r="Q3" s="54"/>
       <c r="R3" s="55"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61">
         <v>2</v>
       </c>
@@ -8299,15 +8311,15 @@
       <c r="D4" s="51">
         <v>1</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="51">
         <v>1</v>
       </c>
       <c r="F4" s="61">
-        <f t="shared" ref="F4:F8" si="0">D4*(C4*30 +E4*30)/60</f>
+        <f t="shared" ref="F4:F7" si="0">D4*(C4*30 +E4*30)/60</f>
         <v>2</v>
       </c>
-      <c r="G4" s="61" t="s">
-        <v>152</v>
+      <c r="G4" s="61">
+        <v>1</v>
       </c>
       <c r="H4" s="69">
         <v>42121</v>
@@ -8334,7 +8346,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="117">
         <v>3</v>
       </c>
@@ -8344,23 +8356,13 @@
       <c r="C5" s="117"/>
       <c r="D5" s="117"/>
       <c r="E5" s="119"/>
-      <c r="F5" s="117">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="117" t="s">
-        <v>152</v>
-      </c>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
       <c r="H5" s="120"/>
       <c r="I5" s="120"/>
       <c r="J5" s="117"/>
-      <c r="K5" s="117" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="121">
-        <f>$O$7*F5</f>
-        <v>0</v>
-      </c>
+      <c r="K5" s="117"/>
+      <c r="L5" s="121"/>
       <c r="N5" s="51" t="s">
         <v>94</v>
       </c>
@@ -8371,7 +8373,7 @@
       <c r="Q5" s="63"/>
       <c r="R5" s="60"/>
     </row>
-    <row r="6" spans="1:18" s="101" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="101" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -8391,7 +8393,9 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="G6" s="87"/>
+      <c r="G6" s="87">
+        <v>4</v>
+      </c>
       <c r="H6" s="69">
         <v>42121</v>
       </c>
@@ -8399,7 +8403,7 @@
         <v>42126</v>
       </c>
       <c r="J6" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K6" s="87"/>
       <c r="L6" s="100"/>
@@ -8408,7 +8412,7 @@
       <c r="Q6" s="105"/>
       <c r="R6" s="106"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="61">
         <v>5</v>
       </c>
@@ -8428,8 +8432,8 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G7" s="61" t="s">
-        <v>152</v>
+      <c r="G7" s="61">
+        <v>19</v>
       </c>
       <c r="H7" s="69">
         <v>42121</v>
@@ -8438,7 +8442,7 @@
         <v>42135</v>
       </c>
       <c r="J7" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K7" s="61" t="s">
         <v>10</v>
@@ -8457,7 +8461,7 @@
       <c r="Q7" s="64"/>
       <c r="R7" s="65"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="117">
         <v>6</v>
       </c>
@@ -8467,27 +8471,17 @@
       <c r="C8" s="117"/>
       <c r="D8" s="117"/>
       <c r="E8" s="119"/>
-      <c r="F8" s="117">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="117" t="s">
-        <v>152</v>
-      </c>
+      <c r="F8" s="117"/>
+      <c r="G8" s="117"/>
       <c r="H8" s="120"/>
       <c r="I8" s="120"/>
       <c r="J8" s="117"/>
-      <c r="K8" s="117" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="121">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K8" s="117"/>
+      <c r="L8" s="121"/>
       <c r="Q8" s="66"/>
       <c r="R8" s="67"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="61">
         <v>7</v>
       </c>
@@ -8500,8 +8494,8 @@
       <c r="F9" s="61">
         <v>2</v>
       </c>
-      <c r="G9" s="61" t="s">
-        <v>152</v>
+      <c r="G9" s="61">
+        <v>2</v>
       </c>
       <c r="H9" s="69">
         <v>42121</v>
@@ -8510,7 +8504,7 @@
         <v>42128</v>
       </c>
       <c r="J9" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K9" s="61"/>
       <c r="L9" s="62">
@@ -8525,7 +8519,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="61">
         <v>8</v>
       </c>
@@ -8538,8 +8532,8 @@
       <c r="F10" s="61">
         <v>2</v>
       </c>
-      <c r="G10" s="61" t="s">
-        <v>152</v>
+      <c r="G10" s="61">
+        <v>3</v>
       </c>
       <c r="H10" s="69">
         <v>42121</v>
@@ -8548,10 +8542,10 @@
         <v>42128</v>
       </c>
       <c r="J10" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K10" s="61" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L10" s="62">
         <f t="shared" si="1"/>
@@ -8564,7 +8558,7 @@
         <v>42091</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="61">
         <v>9</v>
       </c>
@@ -8577,8 +8571,8 @@
       <c r="F11" s="61">
         <v>2</v>
       </c>
-      <c r="G11" s="61" t="s">
-        <v>152</v>
+      <c r="G11" s="61">
+        <v>2</v>
       </c>
       <c r="H11" s="69">
         <v>42121</v>
@@ -8587,10 +8581,10 @@
         <v>42128</v>
       </c>
       <c r="J11" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" s="61" t="s">
         <v>155</v>
-      </c>
-      <c r="K11" s="61" t="s">
-        <v>156</v>
       </c>
       <c r="L11" s="62">
         <f t="shared" si="1"/>
@@ -8603,7 +8597,7 @@
         <v>42098</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="61">
         <v>10</v>
       </c>
@@ -8611,7 +8605,7 @@
         <v>137</v>
       </c>
       <c r="C12" s="61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="61">
         <v>10</v>
@@ -8621,10 +8615,10 @@
       </c>
       <c r="F12" s="56">
         <f>40*C12</f>
-        <v>200</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>152</v>
+        <v>160</v>
+      </c>
+      <c r="G12" s="61">
+        <v>198</v>
       </c>
       <c r="H12" s="69">
         <v>42126</v>
@@ -8636,11 +8630,11 @@
         <v>70</v>
       </c>
       <c r="K12" s="61" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L12" s="62">
         <f t="shared" si="1"/>
-        <v>1411458.3333333335</v>
+        <v>1129166.6666666667</v>
       </c>
       <c r="N12" s="69">
         <v>42100</v>
@@ -8649,7 +8643,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="61">
         <v>11</v>
       </c>
@@ -8662,8 +8656,8 @@
       <c r="F13" s="61">
         <v>3</v>
       </c>
-      <c r="G13" s="61" t="s">
-        <v>152</v>
+      <c r="G13" s="61">
+        <v>3</v>
       </c>
       <c r="H13" s="69">
         <v>42126</v>
@@ -8672,10 +8666,10 @@
         <v>42135</v>
       </c>
       <c r="J13" s="61" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K13" s="61" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="L13" s="62">
         <f t="shared" si="1"/>
@@ -8688,7 +8682,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="61">
         <v>12</v>
       </c>
@@ -8701,8 +8695,8 @@
       <c r="F14" s="61">
         <v>3</v>
       </c>
-      <c r="G14" s="61" t="s">
-        <v>152</v>
+      <c r="G14" s="61">
+        <v>3</v>
       </c>
       <c r="H14" s="69">
         <v>42126</v>
@@ -8727,7 +8721,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117">
         <v>13</v>
       </c>
@@ -8740,8 +8734,8 @@
       <c r="F15" s="117">
         <v>2</v>
       </c>
-      <c r="G15" s="117" t="s">
-        <v>152</v>
+      <c r="G15" s="117">
+        <v>2</v>
       </c>
       <c r="H15" s="132">
         <v>42134</v>
@@ -8766,14 +8760,22 @@
         <v>42126</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="50">
+        <f>SUM(F3:F15)</f>
+        <v>200.5</v>
+      </c>
+      <c r="G16" s="50">
+        <f>SUM(G3:G15)</f>
+        <v>239</v>
+      </c>
       <c r="J16" s="97"/>
       <c r="K16" s="129" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="L16" s="75">
         <f>SUM(L2:L15)</f>
-        <v>1665520.8333333335</v>
+        <v>1383229.1666666667</v>
       </c>
       <c r="N16" s="69">
         <v>42128</v>
@@ -8782,7 +8784,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="97"/>
       <c r="B17" s="108"/>
       <c r="C17" s="97"/>
@@ -8803,7 +8805,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="97"/>
       <c r="B18" s="108"/>
       <c r="C18" s="97"/>
@@ -8824,7 +8826,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="97"/>
       <c r="B19" s="108"/>
       <c r="C19" s="97"/>
@@ -8845,7 +8847,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="97"/>
       <c r="B20" s="108"/>
       <c r="C20" s="97"/>
@@ -8860,7 +8862,7 @@
       <c r="L20" s="111"/>
       <c r="M20" s="78"/>
     </row>
-    <row r="21" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="97"/>
       <c r="B21" s="112"/>
       <c r="C21" s="97"/>
@@ -8875,7 +8877,7 @@
       <c r="L21" s="111"/>
       <c r="M21" s="78"/>
     </row>
-    <row r="22" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="97"/>
       <c r="B22" s="108"/>
       <c r="C22" s="97"/>
@@ -8896,7 +8898,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="97"/>
       <c r="B23" s="108"/>
       <c r="C23" s="97"/>
@@ -8917,7 +8919,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A24" s="97"/>
       <c r="B24" s="108"/>
       <c r="C24" s="97"/>
@@ -8938,7 +8940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="97"/>
       <c r="B25" s="108"/>
       <c r="C25" s="97"/>
@@ -8959,7 +8961,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="97"/>
       <c r="B26" s="108"/>
       <c r="C26" s="97"/>
@@ -8980,7 +8982,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="97"/>
       <c r="B27" s="108"/>
       <c r="C27" s="97"/>
@@ -8995,7 +8997,7 @@
       <c r="L27" s="111"/>
       <c r="M27" s="78"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="97"/>
       <c r="B28" s="108"/>
       <c r="C28" s="97"/>
@@ -9010,7 +9012,7 @@
       <c r="L28" s="111"/>
       <c r="M28" s="78"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="97"/>
       <c r="B29" s="108"/>
       <c r="C29" s="97"/>
@@ -9025,7 +9027,7 @@
       <c r="L29" s="111"/>
       <c r="M29" s="78"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="97"/>
       <c r="B30" s="108"/>
       <c r="C30" s="97"/>
@@ -9040,7 +9042,7 @@
       <c r="L30" s="111"/>
       <c r="M30" s="78"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="97"/>
       <c r="B31" s="108"/>
       <c r="C31" s="97"/>
@@ -9055,7 +9057,7 @@
       <c r="L31" s="111"/>
       <c r="M31" s="78"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="97"/>
       <c r="B32" s="108"/>
       <c r="C32" s="97"/>
@@ -9070,7 +9072,7 @@
       <c r="L32" s="111"/>
       <c r="M32" s="78"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="97"/>
       <c r="B33" s="108"/>
       <c r="C33" s="97"/>
@@ -9085,7 +9087,7 @@
       <c r="L33" s="111"/>
       <c r="M33" s="78"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="97"/>
       <c r="B34" s="108"/>
       <c r="C34" s="97"/>
@@ -9100,7 +9102,7 @@
       <c r="L34" s="111"/>
       <c r="M34" s="78"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="97"/>
       <c r="B35" s="108"/>
       <c r="C35" s="97"/>
@@ -9115,7 +9117,7 @@
       <c r="L35" s="111"/>
       <c r="M35" s="78"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="97"/>
       <c r="B36" s="112"/>
       <c r="C36" s="97"/>
@@ -9130,7 +9132,7 @@
       <c r="L36" s="111"/>
       <c r="M36" s="78"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="97"/>
       <c r="B37" s="108"/>
       <c r="C37" s="97"/>
@@ -9145,7 +9147,7 @@
       <c r="L37" s="111"/>
       <c r="M37" s="78"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="97"/>
       <c r="B38" s="108"/>
       <c r="C38" s="97"/>
@@ -9160,7 +9162,7 @@
       <c r="L38" s="111"/>
       <c r="M38" s="78"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="97"/>
       <c r="B39" s="108"/>
       <c r="C39" s="97"/>
@@ -9175,7 +9177,7 @@
       <c r="L39" s="111"/>
       <c r="M39" s="78"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="97"/>
       <c r="B40" s="108"/>
       <c r="C40" s="97"/>
@@ -9190,7 +9192,7 @@
       <c r="L40" s="111"/>
       <c r="M40" s="78"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="97"/>
       <c r="B41" s="108"/>
       <c r="C41" s="97"/>
@@ -9205,7 +9207,7 @@
       <c r="L41" s="111"/>
       <c r="M41" s="78"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="97"/>
       <c r="B42" s="108"/>
       <c r="C42" s="97"/>
@@ -9220,7 +9222,7 @@
       <c r="L42" s="111"/>
       <c r="M42" s="78"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="97"/>
       <c r="B43" s="108"/>
       <c r="C43" s="97"/>
@@ -9235,7 +9237,7 @@
       <c r="L43" s="111"/>
       <c r="M43" s="78"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="97"/>
       <c r="B44" s="108"/>
       <c r="C44" s="97"/>
@@ -9250,7 +9252,7 @@
       <c r="L44" s="111"/>
       <c r="M44" s="78"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="97"/>
       <c r="B45" s="108"/>
       <c r="C45" s="97"/>
@@ -9265,7 +9267,7 @@
       <c r="L45" s="111"/>
       <c r="M45" s="78"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="97"/>
       <c r="B46" s="108"/>
       <c r="C46" s="97"/>
@@ -9280,7 +9282,7 @@
       <c r="L46" s="111"/>
       <c r="M46" s="78"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="97"/>
       <c r="B47" s="108"/>
       <c r="C47" s="97"/>
@@ -9295,7 +9297,7 @@
       <c r="L47" s="111"/>
       <c r="M47" s="78"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="97"/>
       <c r="B48" s="108"/>
       <c r="C48" s="97"/>
@@ -9310,7 +9312,7 @@
       <c r="L48" s="111"/>
       <c r="M48" s="78"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="97"/>
       <c r="B49" s="112"/>
       <c r="C49" s="97"/>
@@ -9325,7 +9327,7 @@
       <c r="L49" s="111"/>
       <c r="M49" s="78"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="97"/>
       <c r="B50" s="108"/>
       <c r="C50" s="97"/>
@@ -9340,7 +9342,7 @@
       <c r="L50" s="111"/>
       <c r="M50" s="78"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="97"/>
       <c r="B51" s="108"/>
       <c r="C51" s="97"/>
@@ -9355,7 +9357,7 @@
       <c r="L51" s="111"/>
       <c r="M51" s="78"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="97"/>
       <c r="B52" s="108"/>
       <c r="C52" s="97"/>
@@ -9370,7 +9372,7 @@
       <c r="L52" s="111"/>
       <c r="M52" s="78"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="97"/>
       <c r="B53" s="108"/>
       <c r="C53" s="97"/>
@@ -9385,7 +9387,7 @@
       <c r="L53" s="111"/>
       <c r="M53" s="78"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="97"/>
       <c r="B54" s="108"/>
       <c r="C54" s="97"/>
@@ -9400,7 +9402,7 @@
       <c r="L54" s="111"/>
       <c r="M54" s="78"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="97"/>
       <c r="B55" s="108"/>
       <c r="C55" s="97"/>
@@ -9415,7 +9417,7 @@
       <c r="L55" s="111"/>
       <c r="M55" s="78"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="97"/>
       <c r="B56" s="108"/>
       <c r="C56" s="97"/>
@@ -9430,7 +9432,7 @@
       <c r="L56" s="111"/>
       <c r="M56" s="78"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="97"/>
       <c r="B57" s="108"/>
       <c r="C57" s="97"/>
@@ -9445,7 +9447,7 @@
       <c r="L57" s="111"/>
       <c r="M57" s="78"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="97"/>
       <c r="B58" s="108"/>
       <c r="C58" s="97"/>
@@ -9460,7 +9462,7 @@
       <c r="L58" s="111"/>
       <c r="M58" s="78"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="97"/>
       <c r="B59" s="108"/>
       <c r="C59" s="97"/>
@@ -9475,7 +9477,7 @@
       <c r="L59" s="111"/>
       <c r="M59" s="78"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="97"/>
       <c r="B60" s="108"/>
       <c r="C60" s="97"/>
@@ -9490,7 +9492,7 @@
       <c r="L60" s="111"/>
       <c r="M60" s="78"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61" s="97"/>
       <c r="B61" s="108"/>
       <c r="C61" s="97"/>
@@ -9505,7 +9507,7 @@
       <c r="L61" s="111"/>
       <c r="M61" s="78"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="97"/>
       <c r="B62" s="97"/>
       <c r="C62" s="97"/>
@@ -9520,7 +9522,7 @@
       <c r="L62" s="111"/>
       <c r="M62" s="78"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="97"/>
       <c r="B63" s="97"/>
       <c r="C63" s="97"/>
@@ -9535,7 +9537,7 @@
       <c r="L63" s="111"/>
       <c r="M63" s="78"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="97"/>
       <c r="B64" s="97"/>
       <c r="C64" s="97"/>
@@ -9550,7 +9552,7 @@
       <c r="L64" s="111"/>
       <c r="M64" s="78"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="97"/>
       <c r="B65" s="97"/>
       <c r="C65" s="97"/>
@@ -9565,7 +9567,7 @@
       <c r="L65" s="111"/>
       <c r="M65" s="78"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="97"/>
       <c r="B66" s="97"/>
       <c r="C66" s="97"/>
@@ -9580,7 +9582,7 @@
       <c r="L66" s="111"/>
       <c r="M66" s="78"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="97"/>
       <c r="B67" s="97"/>
       <c r="C67" s="97"/>
@@ -9595,7 +9597,7 @@
       <c r="L67" s="111"/>
       <c r="M67" s="78"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="97"/>
       <c r="B68" s="97"/>
       <c r="C68" s="97"/>
@@ -9610,7 +9612,7 @@
       <c r="L68" s="111"/>
       <c r="M68" s="78"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="78"/>
       <c r="B69" s="78"/>
       <c r="K69" s="89" t="s">
@@ -9618,14 +9620,14 @@
       </c>
       <c r="L69" s="90">
         <f>SUM(L62:L68)+L60+L59+L58+L56+L55+L54+L53+L51+L50+L49+L48+L46+L45+L44+L43+L39+L38+L37+L34+L33+L32+L31+L30+L26+L25+L23+L22+L21+L20+L19+SUM(L3:L15)</f>
-        <v>1665520.8333333335</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1383229.1666666667</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
     </row>
@@ -9640,52 +9642,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="133" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="133" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="133" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="133" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="133" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="133" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="133" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="133" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="133" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="133" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="133" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" style="133" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="133" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="133" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="133" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="133" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="133" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="133" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="133" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="133" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="133" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="133" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="133" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="133" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="133" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="133" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="133" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="133" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" style="133" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="133" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="133" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="133" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="133" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="133" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="133" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="133"/>
+    <col min="19" max="16384" width="11.44140625" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="222" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="224" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="223"/>
-      <c r="I1" s="223"/>
-      <c r="J1" s="223"/>
-      <c r="K1" s="223"/>
-      <c r="L1" s="224"/>
-    </row>
-    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="225"/>
+      <c r="J1" s="225"/>
+      <c r="K1" s="225"/>
+      <c r="L1" s="226"/>
+    </row>
+    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="134" t="s">
         <v>0</v>
       </c>
@@ -9729,12 +9731,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="138">
         <v>1</v>
       </c>
       <c r="B3" s="139" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" s="140"/>
       <c r="D3" s="140"/>
@@ -9742,8 +9744,8 @@
       <c r="F3" s="140">
         <v>0.5</v>
       </c>
-      <c r="G3" s="140" t="s">
-        <v>152</v>
+      <c r="G3" s="140">
+        <v>0.2</v>
       </c>
       <c r="H3" s="142">
         <v>42135</v>
@@ -9770,7 +9772,7 @@
       <c r="Q3" s="144"/>
       <c r="R3" s="145"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="146">
         <v>2</v>
       </c>
@@ -9780,24 +9782,13 @@
       <c r="C4" s="146"/>
       <c r="D4" s="146"/>
       <c r="E4" s="148"/>
-      <c r="F4" s="146">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="146" t="s">
-        <v>152</v>
-      </c>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
       <c r="H4" s="149"/>
       <c r="I4" s="149"/>
-      <c r="J4" s="146" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" s="146" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="150">
-        <f>$O$6*F4</f>
-        <v>3528.6458333333335</v>
-      </c>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="150"/>
       <c r="M4" s="151"/>
       <c r="N4" s="140" t="s">
         <v>96</v>
@@ -9808,12 +9799,12 @@
       <c r="Q4" s="153"/>
       <c r="R4" s="154"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="140">
         <v>3</v>
       </c>
       <c r="B5" s="139" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" s="140">
         <v>4</v>
@@ -9821,15 +9812,15 @@
       <c r="D5" s="140">
         <v>2</v>
       </c>
-      <c r="E5" s="141">
+      <c r="E5" s="140">
         <v>2</v>
       </c>
       <c r="F5" s="155">
         <f>D5*(C5*30 +E5*30)/60</f>
         <v>6</v>
       </c>
-      <c r="G5" s="140" t="s">
-        <v>152</v>
+      <c r="G5" s="140">
+        <v>7</v>
       </c>
       <c r="H5" s="142">
         <v>42135</v>
@@ -9858,7 +9849,7 @@
       <c r="Q5" s="157"/>
       <c r="R5" s="154"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="140">
         <v>4</v>
       </c>
@@ -9871,15 +9862,15 @@
       <c r="D6" s="140">
         <v>3</v>
       </c>
-      <c r="E6" s="141">
+      <c r="E6" s="140">
         <v>4</v>
       </c>
       <c r="F6" s="155">
         <f>D6*(C6*30 +E6*30)/60</f>
         <v>21</v>
       </c>
-      <c r="G6" s="140" t="s">
-        <v>152</v>
+      <c r="G6" s="140">
+        <v>25</v>
       </c>
       <c r="H6" s="142">
         <v>42135</v>
@@ -9894,7 +9885,7 @@
         <v>10</v>
       </c>
       <c r="L6" s="143">
-        <f t="shared" ref="L6:L13" si="0">$O$6*F6</f>
+        <f t="shared" ref="L6:L14" si="0">$O$6*F6</f>
         <v>148203.125</v>
       </c>
       <c r="M6" s="151"/>
@@ -9908,7 +9899,7 @@
       <c r="Q6" s="158"/>
       <c r="R6" s="159"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="146">
         <v>5</v>
       </c>
@@ -9919,79 +9910,68 @@
       <c r="D7" s="146"/>
       <c r="E7" s="148"/>
       <c r="F7" s="146"/>
-      <c r="G7" s="146" t="s">
-        <v>152</v>
-      </c>
+      <c r="G7" s="146"/>
       <c r="H7" s="149"/>
       <c r="I7" s="149"/>
-      <c r="J7" s="146" t="s">
-        <v>90</v>
-      </c>
-      <c r="K7" s="146" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="150">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J7" s="146"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="150"/>
       <c r="M7" s="151"/>
       <c r="N7" s="151"/>
       <c r="Q7" s="160"/>
       <c r="R7" s="161"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="214">
         <v>6</v>
       </c>
       <c r="B8" s="162" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="214">
+        <v>4</v>
+      </c>
+      <c r="G8" s="214">
+        <v>4</v>
+      </c>
+      <c r="H8" s="69">
+        <v>42149</v>
+      </c>
+      <c r="I8" s="69">
+        <v>42151</v>
+      </c>
+      <c r="J8" s="214" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="214" t="s">
+        <v>170</v>
+      </c>
+      <c r="L8" s="143">
+        <f>$O$6*F8</f>
+        <v>28229.166666666668</v>
+      </c>
+      <c r="M8" s="151"/>
+      <c r="Q8" s="171"/>
+      <c r="R8" s="171"/>
+    </row>
+    <row r="9" spans="1:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="214">
+        <v>7</v>
+      </c>
+      <c r="B9" s="162" t="s">
         <v>135</v>
-      </c>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="140">
-        <v>2</v>
-      </c>
-      <c r="G8" s="140" t="s">
-        <v>152</v>
-      </c>
-      <c r="H8" s="69">
-        <v>42135</v>
-      </c>
-      <c r="I8" s="69">
-        <v>42139</v>
-      </c>
-      <c r="J8" s="61" t="s">
-        <v>155</v>
-      </c>
-      <c r="K8" s="61"/>
-      <c r="L8" s="143">
-        <f t="shared" si="0"/>
-        <v>14114.583333333334</v>
-      </c>
-      <c r="M8" s="165"/>
-      <c r="N8" s="142">
-        <v>42079</v>
-      </c>
-      <c r="O8" s="156">
-        <v>42084</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="140">
-        <v>7</v>
-      </c>
-      <c r="B9" s="162" t="s">
-        <v>143</v>
       </c>
       <c r="C9" s="140"/>
       <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
+      <c r="E9" s="163"/>
       <c r="F9" s="140">
         <v>2</v>
       </c>
-      <c r="G9" s="140" t="s">
-        <v>152</v>
+      <c r="G9" s="140">
+        <v>2</v>
       </c>
       <c r="H9" s="69">
         <v>42135</v>
@@ -10000,29 +9980,27 @@
         <v>42139</v>
       </c>
       <c r="J9" s="61" t="s">
-        <v>155</v>
-      </c>
-      <c r="K9" s="61" t="s">
-        <v>157</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="K9" s="61"/>
       <c r="L9" s="143">
-        <f t="shared" si="0"/>
+        <f>$O$6*F9</f>
         <v>14114.583333333334</v>
       </c>
-      <c r="M9" s="151"/>
-      <c r="N9" s="166">
-        <v>42086</v>
-      </c>
-      <c r="O9" s="164">
-        <v>42091</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="140">
+      <c r="M9" s="165"/>
+      <c r="N9" s="142">
+        <v>42079</v>
+      </c>
+      <c r="O9" s="156">
+        <v>42084</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="214">
         <v>8</v>
       </c>
       <c r="B10" s="162" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="C10" s="140"/>
       <c r="D10" s="140"/>
@@ -10030,20 +10008,20 @@
       <c r="F10" s="140">
         <v>2</v>
       </c>
-      <c r="G10" s="140" t="s">
-        <v>152</v>
+      <c r="G10" s="140">
+        <v>2</v>
       </c>
       <c r="H10" s="69">
+        <v>42135</v>
+      </c>
+      <c r="I10" s="69">
         <v>42139</v>
       </c>
-      <c r="I10" s="69">
-        <v>42143</v>
-      </c>
       <c r="J10" s="61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K10" s="61" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="L10" s="143">
         <f t="shared" si="0"/>
@@ -10051,109 +10029,105 @@
       </c>
       <c r="M10" s="151"/>
       <c r="N10" s="166">
+        <v>42086</v>
+      </c>
+      <c r="O10" s="164">
+        <v>42091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="214">
+        <v>9</v>
+      </c>
+      <c r="B11" s="162" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140">
+        <v>2</v>
+      </c>
+      <c r="G11" s="140">
+        <v>2</v>
+      </c>
+      <c r="H11" s="69">
+        <v>42139</v>
+      </c>
+      <c r="I11" s="69">
+        <v>42143</v>
+      </c>
+      <c r="J11" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="L11" s="143">
+        <f>$O$6*F11</f>
+        <v>14114.583333333334</v>
+      </c>
+      <c r="M11" s="151"/>
+      <c r="N11" s="166">
         <v>42093</v>
       </c>
-      <c r="O10" s="164">
+      <c r="O11" s="164">
         <v>42098</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="140">
-        <v>9</v>
-      </c>
-      <c r="B11" s="162" t="s">
+    <row r="12" spans="1:18" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="214">
+        <v>10</v>
+      </c>
+      <c r="B12" s="162" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="140">
+      <c r="C12" s="140">
         <v>5</v>
       </c>
-      <c r="D11" s="140">
+      <c r="D12" s="140">
         <v>10</v>
       </c>
-      <c r="E11" s="140">
+      <c r="E12" s="140">
         <v>0</v>
       </c>
-      <c r="F11" s="56">
-        <f>40*C11</f>
+      <c r="F12" s="56">
+        <f>40*C12</f>
         <v>200</v>
       </c>
-      <c r="G11" s="140" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" s="69">
+      <c r="G12" s="140">
+        <v>200</v>
+      </c>
+      <c r="H12" s="69">
         <v>42135</v>
       </c>
-      <c r="I11" s="69">
+      <c r="I12" s="69">
         <v>42151</v>
       </c>
-      <c r="J11" s="61" t="s">
+      <c r="J12" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="L11" s="143">
+      <c r="K12" s="61" t="s">
+        <v>171</v>
+      </c>
+      <c r="L12" s="143">
         <f t="shared" si="0"/>
         <v>1411458.3333333335</v>
       </c>
-      <c r="M11" s="151"/>
-      <c r="N11" s="166">
-        <v>42100</v>
-      </c>
-      <c r="O11" s="164">
-        <v>42105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="140">
-        <v>10</v>
-      </c>
-      <c r="B12" s="162" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140">
-        <v>3</v>
-      </c>
-      <c r="G12" s="140" t="s">
-        <v>152</v>
-      </c>
-      <c r="H12" s="69">
-        <v>42143</v>
-      </c>
-      <c r="I12" s="52">
-        <v>42152</v>
-      </c>
-      <c r="J12" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="K12" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="L12" s="143">
-        <f t="shared" si="0"/>
-        <v>21171.875</v>
-      </c>
       <c r="M12" s="151"/>
       <c r="N12" s="166">
-        <v>42107</v>
+        <v>42100</v>
       </c>
       <c r="O12" s="164">
-        <v>42112</v>
-      </c>
-      <c r="R12" s="199">
-        <f>O4*7</f>
-        <v>11856250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="140">
+        <v>42105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="214">
         <v>11</v>
       </c>
       <c r="B13" s="162" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="140"/>
       <c r="D13" s="140"/>
@@ -10161,8 +10135,8 @@
       <c r="F13" s="140">
         <v>3</v>
       </c>
-      <c r="G13" s="140" t="s">
-        <v>152</v>
+      <c r="G13" s="140">
+        <v>3</v>
       </c>
       <c r="H13" s="69">
         <v>42143</v>
@@ -10171,10 +10145,10 @@
         <v>42152</v>
       </c>
       <c r="J13" s="61" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="K13" s="61" t="s">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="L13" s="143">
         <f t="shared" si="0"/>
@@ -10182,97 +10156,128 @@
       </c>
       <c r="M13" s="151"/>
       <c r="N13" s="166">
-        <v>42114</v>
+        <v>42107</v>
       </c>
       <c r="O13" s="164">
-        <v>42119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="146">
+        <v>42112</v>
+      </c>
+      <c r="R13" s="199">
+        <f>O4*7</f>
+        <v>11856250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="214">
         <v>12</v>
       </c>
-      <c r="B14" s="147" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="146">
-        <v>5</v>
-      </c>
-      <c r="D14" s="146">
-        <v>5</v>
-      </c>
-      <c r="E14" s="148">
-        <v>5</v>
-      </c>
-      <c r="F14" s="146">
-        <f>D14*(C14*30 +E14*30)/60</f>
-        <v>25</v>
-      </c>
-      <c r="G14" s="146" t="s">
-        <v>152</v>
-      </c>
-      <c r="H14" s="132">
+      <c r="B14" s="162" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="140"/>
+      <c r="D14" s="140"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="140">
+        <v>3</v>
+      </c>
+      <c r="G14" s="140">
+        <v>3</v>
+      </c>
+      <c r="H14" s="69">
+        <v>42143</v>
+      </c>
+      <c r="I14" s="52">
         <v>42152</v>
       </c>
-      <c r="I14" s="132">
-        <v>42153</v>
-      </c>
-      <c r="J14" s="146" t="s">
-        <v>90</v>
-      </c>
-      <c r="K14" s="146" t="s">
+      <c r="J14" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="150">
-        <f>$O$6*F14</f>
-        <v>176432.29166666669</v>
+      <c r="L14" s="143">
+        <f t="shared" si="0"/>
+        <v>21171.875</v>
       </c>
       <c r="M14" s="151"/>
       <c r="N14" s="166">
-        <v>42121</v>
+        <v>42114</v>
       </c>
       <c r="O14" s="164">
-        <v>42126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K15" s="167" t="s">
-        <v>163</v>
-      </c>
-      <c r="L15" s="168">
-        <f>SUM(L1:L14)</f>
-        <v>1870182.291666667</v>
+        <v>42119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="146">
+        <v>13</v>
+      </c>
+      <c r="B15" s="147" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="146">
+        <v>5</v>
+      </c>
+      <c r="D15" s="146">
+        <v>5</v>
+      </c>
+      <c r="E15" s="146">
+        <v>5</v>
+      </c>
+      <c r="F15" s="146">
+        <f>D15*(C15*30 +E15*30)/60</f>
+        <v>25</v>
+      </c>
+      <c r="G15" s="146">
+        <v>25</v>
+      </c>
+      <c r="H15" s="132">
+        <v>42152</v>
+      </c>
+      <c r="I15" s="132">
+        <v>42153</v>
+      </c>
+      <c r="J15" s="146" t="s">
+        <v>90</v>
+      </c>
+      <c r="K15" s="146" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="150">
+        <f>$O$6*F15</f>
+        <v>176432.29166666669</v>
       </c>
       <c r="M15" s="151"/>
       <c r="N15" s="166">
+        <v>42121</v>
+      </c>
+      <c r="O15" s="164">
+        <v>42126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="133">
+        <f>SUM(F3:F15)</f>
+        <v>268.5</v>
+      </c>
+      <c r="G16" s="133">
+        <f>SUM(G3:G15)</f>
+        <v>273.2</v>
+      </c>
+      <c r="K16" s="167" t="s">
+        <v>173</v>
+      </c>
+      <c r="L16" s="168">
+        <f>SUM(L1:L15)</f>
+        <v>1894882.8125000002</v>
+      </c>
+      <c r="M16" s="151"/>
+      <c r="N16" s="166">
         <v>42128</v>
       </c>
-      <c r="O15" s="164">
+      <c r="O16" s="164">
         <v>42133</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="171"/>
-      <c r="B16" s="172"/>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="173"/>
-      <c r="F16" s="171"/>
-      <c r="G16" s="171"/>
-      <c r="H16" s="174"/>
-      <c r="I16" s="174"/>
-      <c r="J16" s="171"/>
-      <c r="K16" s="171"/>
-      <c r="L16" s="175"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="177">
-        <v>42135</v>
-      </c>
-      <c r="O16" s="156">
-        <v>42140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="171"/>
       <c r="B17" s="172"/>
       <c r="C17" s="171"/>
@@ -10286,14 +10291,14 @@
       <c r="K17" s="171"/>
       <c r="L17" s="175"/>
       <c r="M17" s="176"/>
-      <c r="N17" s="178">
-        <v>42142</v>
-      </c>
-      <c r="O17" s="164">
-        <v>42147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="177">
+        <v>42135</v>
+      </c>
+      <c r="O17" s="156">
+        <v>42140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="171"/>
       <c r="B18" s="172"/>
       <c r="C18" s="171"/>
@@ -10308,13 +10313,13 @@
       <c r="L18" s="175"/>
       <c r="M18" s="176"/>
       <c r="N18" s="178">
-        <v>42149</v>
+        <v>42142</v>
       </c>
       <c r="O18" s="164">
-        <v>42154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>42147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="171"/>
       <c r="B19" s="172"/>
       <c r="C19" s="171"/>
@@ -10328,9 +10333,14 @@
       <c r="K19" s="171"/>
       <c r="L19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="N19" s="176"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="178">
+        <v>42149</v>
+      </c>
+      <c r="O19" s="164">
+        <v>42154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="171"/>
       <c r="B20" s="172"/>
       <c r="C20" s="171"/>
@@ -10346,7 +10356,7 @@
       <c r="M20" s="176"/>
       <c r="N20" s="176"/>
     </row>
-    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="171"/>
       <c r="B21" s="172"/>
       <c r="C21" s="171"/>
@@ -10360,14 +10370,9 @@
       <c r="K21" s="171"/>
       <c r="L21" s="175"/>
       <c r="M21" s="176"/>
-      <c r="N21" s="179" t="s">
-        <v>77</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="176"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="171"/>
       <c r="B22" s="172"/>
       <c r="C22" s="171"/>
@@ -10381,14 +10386,14 @@
       <c r="K22" s="171"/>
       <c r="L22" s="175"/>
       <c r="M22" s="176"/>
-      <c r="N22" s="180" t="s">
-        <v>70</v>
-      </c>
-      <c r="O22" s="145" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="179" t="s">
+        <v>77</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="171"/>
       <c r="B23" s="172"/>
       <c r="C23" s="171"/>
@@ -10402,14 +10407,14 @@
       <c r="K23" s="171"/>
       <c r="L23" s="175"/>
       <c r="M23" s="176"/>
-      <c r="N23" s="181" t="s">
-        <v>74</v>
-      </c>
-      <c r="O23" s="169" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="180" t="s">
+        <v>70</v>
+      </c>
+      <c r="O23" s="145" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="171"/>
       <c r="B24" s="172"/>
       <c r="C24" s="171"/>
@@ -10424,13 +10429,13 @@
       <c r="L24" s="175"/>
       <c r="M24" s="176"/>
       <c r="N24" s="181" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O24" s="169" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="171"/>
       <c r="B25" s="172"/>
       <c r="C25" s="171"/>
@@ -10444,14 +10449,14 @@
       <c r="K25" s="171"/>
       <c r="L25" s="175"/>
       <c r="M25" s="176"/>
-      <c r="N25" s="182" t="s">
-        <v>84</v>
-      </c>
-      <c r="O25" s="170" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N25" s="181" t="s">
+        <v>76</v>
+      </c>
+      <c r="O25" s="169" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="171"/>
       <c r="B26" s="172"/>
       <c r="C26" s="171"/>
@@ -10465,9 +10470,14 @@
       <c r="K26" s="171"/>
       <c r="L26" s="175"/>
       <c r="M26" s="176"/>
-      <c r="N26" s="176"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N26" s="182" t="s">
+        <v>84</v>
+      </c>
+      <c r="O26" s="170" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="171"/>
       <c r="B27" s="172"/>
       <c r="C27" s="171"/>
@@ -10483,7 +10493,7 @@
       <c r="M27" s="176"/>
       <c r="N27" s="176"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="171"/>
       <c r="B28" s="172"/>
       <c r="C28" s="171"/>
@@ -10499,12 +10509,12 @@
       <c r="M28" s="176"/>
       <c r="N28" s="176"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="171"/>
       <c r="B29" s="172"/>
       <c r="C29" s="171"/>
       <c r="D29" s="171"/>
-      <c r="E29" s="183"/>
+      <c r="E29" s="173"/>
       <c r="F29" s="171"/>
       <c r="G29" s="171"/>
       <c r="H29" s="174"/>
@@ -10517,21 +10527,21 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="171"/>
-      <c r="B30" s="171"/>
+      <c r="B30" s="172"/>
       <c r="C30" s="171"/>
       <c r="D30" s="171"/>
-      <c r="E30" s="171"/>
+      <c r="E30" s="183"/>
       <c r="F30" s="171"/>
       <c r="G30" s="171"/>
-      <c r="H30" s="171"/>
-      <c r="I30" s="171"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="174"/>
       <c r="J30" s="171"/>
       <c r="K30" s="171"/>
       <c r="L30" s="175"/>
       <c r="M30" s="176"/>
       <c r="N30" s="176"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="171"/>
       <c r="B31" s="171"/>
       <c r="C31" s="171"/>
@@ -10547,7 +10557,7 @@
       <c r="M31" s="176"/>
       <c r="N31" s="176"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="171"/>
       <c r="B32" s="171"/>
       <c r="C32" s="171"/>
@@ -10563,7 +10573,7 @@
       <c r="M32" s="176"/>
       <c r="N32" s="176"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="171"/>
       <c r="B33" s="171"/>
       <c r="C33" s="171"/>
@@ -10579,7 +10589,7 @@
       <c r="M33" s="176"/>
       <c r="N33" s="176"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="171"/>
       <c r="B34" s="171"/>
       <c r="C34" s="171"/>
@@ -10595,7 +10605,7 @@
       <c r="M34" s="176"/>
       <c r="N34" s="176"/>
     </row>
-    <row r="35" spans="1:14" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="171"/>
       <c r="B35" s="171"/>
       <c r="C35" s="171"/>
@@ -10611,7 +10621,7 @@
       <c r="M35" s="176"/>
       <c r="N35" s="176"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="171"/>
       <c r="B36" s="171"/>
       <c r="C36" s="171"/>
@@ -10627,7 +10637,7 @@
       <c r="M36" s="176"/>
       <c r="N36" s="176"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="171"/>
       <c r="B37" s="171"/>
       <c r="C37" s="171"/>
@@ -10639,11 +10649,11 @@
       <c r="I37" s="171"/>
       <c r="J37" s="171"/>
       <c r="K37" s="171"/>
-      <c r="L37" s="184"/>
+      <c r="L37" s="175"/>
       <c r="M37" s="176"/>
       <c r="N37" s="176"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="171"/>
       <c r="B38" s="171"/>
       <c r="C38" s="171"/>
@@ -10655,11 +10665,11 @@
       <c r="I38" s="171"/>
       <c r="J38" s="171"/>
       <c r="K38" s="171"/>
-      <c r="L38" s="171"/>
+      <c r="L38" s="184"/>
       <c r="M38" s="176"/>
       <c r="N38" s="176"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="171"/>
       <c r="B39" s="171"/>
       <c r="C39" s="171"/>
@@ -10675,7 +10685,7 @@
       <c r="M39" s="176"/>
       <c r="N39" s="176"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="171"/>
       <c r="B40" s="171"/>
       <c r="C40" s="171"/>
@@ -10691,129 +10701,145 @@
       <c r="M40" s="176"/>
       <c r="N40" s="176"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="171"/>
+      <c r="B41" s="171"/>
+      <c r="C41" s="171"/>
+      <c r="D41" s="171"/>
+      <c r="E41" s="171"/>
+      <c r="F41" s="171"/>
+      <c r="G41" s="171"/>
+      <c r="H41" s="171"/>
+      <c r="I41" s="171"/>
+      <c r="J41" s="171"/>
+      <c r="K41" s="171"/>
+      <c r="L41" s="171"/>
+      <c r="M41" s="176"/>
       <c r="N41" s="176"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="171"/>
       <c r="N42" s="176"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="171"/>
       <c r="N43" s="176"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="171"/>
       <c r="N44" s="176"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="171"/>
       <c r="N45" s="176"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="171"/>
       <c r="N46" s="176"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="171"/>
       <c r="N47" s="176"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="171"/>
       <c r="N48" s="176"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="171"/>
       <c r="N49" s="176"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="171"/>
       <c r="N50" s="176"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="171"/>
       <c r="N51" s="176"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="171"/>
       <c r="N52" s="176"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="171"/>
       <c r="N53" s="176"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="171"/>
       <c r="N54" s="176"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="171"/>
       <c r="N55" s="176"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="171"/>
       <c r="N56" s="176"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="171"/>
       <c r="N57" s="176"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="171"/>
       <c r="N58" s="176"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="171"/>
       <c r="N59" s="176"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="171"/>
       <c r="N60" s="176"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="171"/>
       <c r="N61" s="176"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="171"/>
       <c r="N62" s="176"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="171"/>
       <c r="N63" s="176"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="171"/>
       <c r="N64" s="176"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="171"/>
       <c r="N65" s="176"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="171"/>
       <c r="N66" s="176"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="171"/>
       <c r="N67" s="176"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="171"/>
       <c r="N68" s="176"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="171"/>
       <c r="N69" s="176"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="171"/>
       <c r="N70" s="176"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="171"/>
       <c r="N71" s="176"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72" s="171"/>
+      <c r="N72" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>